<commit_message>
updated traits table to include personalityType for referencing to personalities table
</commit_message>
<xml_diff>
--- a/Database/Traits.xlsx
+++ b/Database/Traits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zihui/Documents/GitHub/DIP-Group-6-Android/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08111AF7-9984-DC4E-9DF5-7BA6B013D1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D699A1E3-2134-9346-847C-3BC9994872E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{B5778CAD-5055-B24B-A4AA-D8AAAB6BE1AD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
   <si>
     <t>PriId</t>
   </si>
@@ -44,9 +44,6 @@
     <t>QuizCategory</t>
   </si>
   <si>
-    <t>Trait</t>
-  </si>
-  <si>
     <t>Desc</t>
   </si>
   <si>
@@ -201,13 +198,67 @@
   </si>
   <si>
     <t>You set goals that are attainable for you/your team. You always aim for the best results given the current situation.</t>
+  </si>
+  <si>
+    <t>PersonalityType</t>
+  </si>
+  <si>
+    <t>TraitName</t>
+  </si>
+  <si>
+    <t>ENTJ</t>
+  </si>
+  <si>
+    <t>EOTJ</t>
+  </si>
+  <si>
+    <t>ENPJ</t>
+  </si>
+  <si>
+    <t>EOPJ</t>
+  </si>
+  <si>
+    <t>ENTF</t>
+  </si>
+  <si>
+    <t>EOTF</t>
+  </si>
+  <si>
+    <t>ENPF</t>
+  </si>
+  <si>
+    <t>EOPF</t>
+  </si>
+  <si>
+    <t>INTJ</t>
+  </si>
+  <si>
+    <t>IOTJ</t>
+  </si>
+  <si>
+    <t>INPJ</t>
+  </si>
+  <si>
+    <t>IOPJ</t>
+  </si>
+  <si>
+    <t>INTF</t>
+  </si>
+  <si>
+    <t>IOTF</t>
+  </si>
+  <si>
+    <t>INPF</t>
+  </si>
+  <si>
+    <t>IOPF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -227,6 +278,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -249,11 +308,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,369 +628,444 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D92400F-BB37-2543-A91A-B22626F9B8B9}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="132.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="132.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>